<commit_message>
Updated README with how to parse xlsx to json. Updated seals.
</commit_message>
<xml_diff>
--- a/app/data/Sälar.xlsx
+++ b/app/data/Sälar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\workspace\web\sealsofnordigt\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\OneDrive\Dokument\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sälbeskrivning" sheetId="3" r:id="rId2"/>
     <sheet name="Avsnitt" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
   <si>
     <t>Avsnitt</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Halv SÄL</t>
   </si>
   <si>
-    <t>TWD</t>
-  </si>
-  <si>
     <t>Malin Söderberg</t>
   </si>
   <si>
@@ -151,6 +148,75 @@
     <t>POTENTIÄL</t>
   </si>
   <si>
+    <t>ZÄL</t>
+  </si>
+  <si>
+    <t>EP131</t>
+  </si>
+  <si>
+    <t>Dying light</t>
+  </si>
+  <si>
+    <t>Zombie-säl</t>
+  </si>
+  <si>
+    <t>MATS-SÄL</t>
+  </si>
+  <si>
+    <t>American Truck Simulator</t>
+  </si>
+  <si>
+    <t>Marvelsäl</t>
+  </si>
+  <si>
+    <t>EP130</t>
+  </si>
+  <si>
+    <t>Deadpool</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>Lady killer</t>
+  </si>
+  <si>
+    <t>Strange empires</t>
+  </si>
+  <si>
+    <t>GOTY/SÄL</t>
+  </si>
+  <si>
+    <t>Xcom 2</t>
+  </si>
+  <si>
+    <t>Mats/Niklas</t>
+  </si>
+  <si>
+    <t>DCSÄL</t>
+  </si>
+  <si>
+    <t>EP133</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Sälunderhot</t>
+  </si>
+  <si>
+    <t>Victor (Vanne)</t>
+  </si>
+  <si>
+    <t>EP135</t>
+  </si>
+  <si>
+    <t>House of cards</t>
+  </si>
+  <si>
+    <t>Niklas/Tove</t>
+  </si>
+  <si>
     <t>KÄL</t>
   </si>
   <si>
@@ -166,6 +232,18 @@
     <t>Myntades av lyssnare, När man inte kan komma överens om vad för säl något ska få</t>
   </si>
   <si>
+    <t>Zombiesäl</t>
+  </si>
+  <si>
+    <t>Vanne</t>
+  </si>
+  <si>
+    <t>Motsvarighet till marvelsäl</t>
+  </si>
+  <si>
+    <t>Säl som hotats fram av annan panelmedlem, tyck som jag annars...</t>
+  </si>
+  <si>
     <t>EP116</t>
   </si>
   <si>
@@ -196,28 +274,130 @@
     <t>EP127</t>
   </si>
   <si>
+    <t>EP128</t>
+  </si>
+  <si>
+    <t>EP129</t>
+  </si>
+  <si>
+    <t>EP132</t>
+  </si>
+  <si>
+    <t>EP134</t>
+  </si>
+  <si>
+    <t>EP136</t>
+  </si>
+  <si>
+    <t>EP137</t>
+  </si>
+  <si>
+    <t>EP138</t>
+  </si>
+  <si>
+    <t>EP139</t>
+  </si>
+  <si>
+    <t>EP140</t>
+  </si>
+  <si>
+    <t>EP141</t>
+  </si>
+  <si>
+    <t>EP142</t>
+  </si>
+  <si>
+    <t>EP143</t>
+  </si>
+  <si>
+    <t>EP144</t>
+  </si>
+  <si>
+    <t>EP145</t>
+  </si>
+  <si>
+    <t>EP146</t>
+  </si>
+  <si>
+    <t>EP147</t>
+  </si>
+  <si>
+    <t>EP148</t>
+  </si>
+  <si>
+    <t>EP149</t>
+  </si>
+  <si>
+    <t>EP150</t>
+  </si>
+  <si>
+    <t>EP151</t>
+  </si>
+  <si>
+    <t>EP152</t>
+  </si>
+  <si>
+    <t>EP153</t>
+  </si>
+  <si>
+    <t>EP154</t>
+  </si>
+  <si>
+    <t>EP155</t>
+  </si>
+  <si>
+    <t>EP156</t>
+  </si>
+  <si>
+    <t>The Division</t>
+  </si>
+  <si>
+    <t>(Otydligsäl?)</t>
+  </si>
+  <si>
+    <t>Heavy Rain Remastered</t>
+  </si>
+  <si>
+    <t>Tove, Mats, Niklas, Peter</t>
+  </si>
+  <si>
+    <t>Daredevil S02</t>
+  </si>
+  <si>
+    <t>Sympatisäl</t>
+  </si>
+  <si>
+    <t>Batman v Superman</t>
+  </si>
+  <si>
+    <t>The Walking Dead</t>
+  </si>
+  <si>
     <t>Star Wars VII: The Force Awakens</t>
   </si>
   <si>
     <t>Tove, Mats, Peter, Jonas, Niklas, Vanne, Viktor</t>
   </si>
   <si>
+    <t>seal</t>
+  </si>
+  <si>
+    <t>episode</t>
+  </si>
+  <si>
     <t>titel</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>episode</t>
-  </si>
-  <si>
-    <t>seal</t>
-  </si>
-  <si>
     <t>publisher</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -247,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +454,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFAC08F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -354,6 +540,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dekorfärg1" xfId="1" builtinId="29"/>
@@ -448,6 +636,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -483,6 +688,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -635,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A2:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,287 +868,548 @@
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="C27" t="s">
         <v>57</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -936,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C7"/>
+  <dimension ref="A3:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,50 +1430,92 @@
     <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1001,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,38 +1545,38 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1061,27 +1586,172 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>34</v>
+      <c r="A12" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>